<commit_message>
Category model 삭제 (Store model에 통합)
</commit_message>
<xml_diff>
--- a/crawling/data/yogiyo_서울대_final.xlsx
+++ b/crawling/data/yogiyo_서울대_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\error_fix\crawling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E986B5F-8A3E-4491-B01B-406ED44CF60C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09327B5C-8FFE-4FC9-9866-9C31F704BA68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="치킨" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4861" uniqueCount="1946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4874" uniqueCount="1947">
   <si>
     <t>상세페이지URL</t>
   </si>
@@ -5874,6 +5874,10 @@
   </si>
   <si>
     <t>테트리스찜닭-관악점</t>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6243,8 +6247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -8599,7 +8603,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -8637,13 +8641,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41A7A93-EC7F-48E6-AF5C-3C4F0B96B6AA}">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="H97" sqref="H97"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="3" max="3" width="49.625" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -9536,6 +9541,9 @@
       <c r="E39" t="s">
         <v>27</v>
       </c>
+      <c r="F39" t="s">
+        <v>1946</v>
+      </c>
       <c r="G39" s="1">
         <v>123</v>
       </c>
@@ -9786,6 +9794,9 @@
       <c r="E50" t="s">
         <v>231</v>
       </c>
+      <c r="F50" t="s">
+        <v>1946</v>
+      </c>
       <c r="G50" s="1">
         <v>59</v>
       </c>
@@ -10266,6 +10277,9 @@
       <c r="E71" t="s">
         <v>27</v>
       </c>
+      <c r="F71" t="s">
+        <v>1946</v>
+      </c>
       <c r="G71" s="1">
         <v>17</v>
       </c>
@@ -10809,8 +10823,14 @@
       <c r="C95" t="s">
         <v>525</v>
       </c>
+      <c r="D95" s="2" t="s">
+        <v>1946</v>
+      </c>
       <c r="E95" t="s">
         <v>87</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>1946</v>
       </c>
       <c r="G95" s="1">
         <v>0</v>
@@ -10826,8 +10846,14 @@
       <c r="C96" t="s">
         <v>527</v>
       </c>
+      <c r="D96" s="2" t="s">
+        <v>1946</v>
+      </c>
       <c r="E96" t="s">
         <v>57</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>1946</v>
       </c>
       <c r="G96" s="1">
         <v>0</v>
@@ -10843,8 +10869,14 @@
       <c r="C97" t="s">
         <v>530</v>
       </c>
+      <c r="D97" s="2" t="s">
+        <v>1946</v>
+      </c>
       <c r="E97" t="s">
         <v>51</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>1946</v>
       </c>
       <c r="G97" s="1">
         <v>0</v>
@@ -10860,8 +10892,14 @@
       <c r="C98" t="s">
         <v>590</v>
       </c>
+      <c r="D98" s="2" t="s">
+        <v>1946</v>
+      </c>
       <c r="E98" t="s">
         <v>591</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>1946</v>
       </c>
       <c r="G98" s="1">
         <v>0</v>
@@ -10877,8 +10915,14 @@
       <c r="C99" t="s">
         <v>594</v>
       </c>
+      <c r="D99" t="s">
+        <v>1946</v>
+      </c>
       <c r="E99" t="s">
         <v>231</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>1946</v>
       </c>
       <c r="G99" s="1">
         <v>0</v>
@@ -11050,8 +11094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91B29A1-09AF-4042-A7BE-1878BB72E077}">
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -12522,8 +12566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38BCA0A-C8D2-4C36-8BA6-56D5938B9E0F}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView topLeftCell="B73" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -14870,8 +14914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1042010A-678A-49CA-867C-B98715D04A6B}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="H102" sqref="H102"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -17216,8 +17260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C188D7-9066-4A10-AD25-75BE3143D94A}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -19045,8 +19089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0187EE52-2FD8-4DCA-A004-843989572EB3}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -21401,7 +21445,7 @@
   <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="J122" sqref="J122"/>
+      <selection activeCell="A2" sqref="A2:G121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -24287,8 +24331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF62A510-41CA-4CA8-B2C8-131B2D4B0A88}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>